<commit_message>
archivos inutiles eliminados y nombres estandar
</commit_message>
<xml_diff>
--- a/COSTOS_INDIRECTOS_DE_ESTUDIO_PROF_2025_COMPLETO.xlsx
+++ b/COSTOS_INDIRECTOS_DE_ESTUDIO_PROF_2025_COMPLETO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D7A348A-6456-4289-8E2C-763DBECE1CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5DE0135-3C71-4351-8741-349F9E3F6708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Detalle</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>3.10 Backup en la nube (fijo)</t>
+  </si>
+  <si>
+    <t>(8 empleados)</t>
   </si>
 </sst>
 </file>
@@ -647,10 +650,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -659,6 +662,7 @@
     <col min="2" max="2" width="28" customWidth="1"/>
     <col min="3" max="3" width="25.33203125" customWidth="1"/>
     <col min="4" max="5" width="22" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -736,11 +740,11 @@
       <c r="B6" s="3"/>
       <c r="C6" s="2"/>
       <c r="D6" s="3">
-        <v>960000</v>
+        <v>3600000</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" si="0"/>
-        <v>80000</v>
+        <f>D6/12</f>
+        <v>300000</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -750,11 +754,11 @@
       <c r="B7" s="3"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3">
-        <v>25200</v>
+        <v>360000</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" si="0"/>
-        <v>2100</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -908,7 +912,7 @@
         <v>1111.1111111111111</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
@@ -927,7 +931,7 @@
         <v>2666.6666666666665</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>31</v>
       </c>
@@ -946,7 +950,7 @@
         <v>16666.666666666668</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>30</v>
       </c>
@@ -965,7 +969,7 @@
         <v>12500</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
@@ -979,7 +983,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -993,7 +997,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
@@ -1007,7 +1011,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
@@ -1021,7 +1025,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>44</v>
       </c>
@@ -1035,7 +1039,7 @@
         <v>25000</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="15" t="s">
         <v>14</v>
       </c>
@@ -1044,7 +1048,7 @@
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>15</v>
       </c>
@@ -1058,7 +1062,7 @@
         <v>52500</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>29</v>
       </c>
@@ -1072,7 +1076,7 @@
         <v>29166.666666666668</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>20</v>
       </c>
@@ -1081,38 +1085,40 @@
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="9">
-        <v>440000</v>
+        <v>1355000</v>
       </c>
       <c r="E29" s="9">
         <f>D29/12</f>
-        <v>36666.666666666664</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <v>112916.66666666667</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B30" s="2">
-        <v>300</v>
+      <c r="B30" s="9">
+        <v>2700</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="9">
-        <f>(B30*8)*12</f>
-        <v>28800</v>
+        <v>259200</v>
       </c>
       <c r="E30" s="9">
         <f t="shared" ref="E30:E31" si="4">D30/12</f>
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+        <v>21600</v>
+      </c>
+      <c r="F30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>23</v>
       </c>
@@ -1126,7 +1132,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="15" t="s">
         <v>26</v>
       </c>
@@ -1156,11 +1162,11 @@
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
       <c r="D34" s="9">
-        <v>100000</v>
+        <v>1370000</v>
       </c>
       <c r="E34" s="9">
         <f>D34/12</f>
-        <v>8333.3333333333339</v>
+        <v>114166.66666666667</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1179,11 +1185,11 @@
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9">
-        <v>200000</v>
+        <v>2160000</v>
       </c>
       <c r="E36" s="9">
         <f>D36/12</f>
-        <v>16666.666666666668</v>
+        <v>180000</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1201,7 +1207,7 @@
       </c>
       <c r="D38" s="5">
         <f>SUM(D2:D37)</f>
-        <v>21690666.666666668</v>
+        <v>29040866.666666668</v>
       </c>
       <c r="E38" s="6"/>
     </row>
@@ -1212,7 +1218,7 @@
       <c r="D39" s="6"/>
       <c r="E39" s="5">
         <f>SUM(E2:E37)</f>
-        <v>1807555.5555555557</v>
+        <v>2420072.2222222225</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1222,7 +1228,7 @@
       <c r="D40" s="6"/>
       <c r="E40" s="6">
         <f>E39/30</f>
-        <v>60251.851851851861</v>
+        <v>80669.074074074088</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1234,7 +1240,7 @@
       </c>
       <c r="E41" s="7">
         <f>D41*E40</f>
-        <v>2575766.666666667</v>
+        <v>3448602.9166666674</v>
       </c>
     </row>
   </sheetData>

</xml_diff>